<commit_message>
Update to current US develop branch
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66582C1F-0C47-42E5-9226-B6D9CE2514BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502B28A-161E-4459-AD22-FA23663F12B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Source:</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>This is a Boolean value that should be set to 0 or 1 in each year.</t>
-  </si>
-  <si>
-    <t>2028 and new combined cycle gas without CCS is banned starting in 2032.</t>
   </si>
   <si>
     <t>In the U.S., we use this to represent EPA 111 Rules. New coal without CCS is banned starting in</t>
@@ -523,7 +520,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,12 +573,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
+      <c r="A13">
+        <v>2028</v>
       </c>
     </row>
   </sheetData>
@@ -597,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:AE14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,61 +927,61 @@
         <v>0</v>
       </c>
       <c r="M4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to official main branch of eps-us, tag 4.0.0.1
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502B28A-161E-4459-AD22-FA23663F12B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7697ECBD-92C9-4103-9555-181ACE6C7B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:AE4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,13 +704,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -799,13 +799,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -894,13 +894,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -989,13 +989,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1084,13 +1084,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1274,13 +1274,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1369,13 +1369,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1464,13 +1464,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1559,13 +1559,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1654,13 +1654,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1749,13 +1749,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1844,13 +1844,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1939,13 +1939,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2034,13 +2034,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2129,13 +2129,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2224,13 +2224,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2319,13 +2319,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
@@ -2414,13 +2414,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
@@ -2509,13 +2509,13 @@
         <v>22</v>
       </c>
       <c r="B21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -2604,13 +2604,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -2699,13 +2699,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2794,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2889,13 +2889,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Updates to eps-us commit #54625f6
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7CBECA-90CF-4BE3-9075-5F308FED293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327A7F1-3EF2-40B1-8B65-730CF1661ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1455" windowWidth="27360" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -610,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,13 +720,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1005,13 +1005,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1100,13 +1100,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1195,13 +1195,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1290,13 +1290,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1385,13 +1385,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1480,13 +1480,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1575,13 +1575,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1670,13 +1670,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1765,13 +1765,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1860,13 +1860,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1955,13 +1955,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2050,13 +2050,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2145,13 +2145,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2240,13 +2240,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2715,13 +2715,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2810,13 +2810,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2905,13 +2905,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Use BAU BECCS ban rather than policy lever to remove it from wedge diagram.
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49442315-96A3-4B7D-8461-0B069A837438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E195D9-0360-4576-AA72-E7FBED472E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57780" yWindow="570" windowWidth="28620" windowHeight="16620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33585" yWindow="1950" windowWidth="21870" windowHeight="13605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -557,8 +557,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:AE25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2472,94 +2472,94 @@
         <v>22</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updates to eps-us commit #8780d0b
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327A7F1-3EF2-40B1-8B65-730CF1661ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5C7C3-C6DD-4CC0-A75D-D5DA17DC76DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38865" windowHeight="17235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B2" sqref="B2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,14 +719,14 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -814,14 +814,14 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -909,14 +909,14 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1004,14 +1004,14 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1099,14 +1099,14 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1194,14 +1194,14 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1289,14 +1289,14 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1384,14 +1384,14 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1479,14 +1479,14 @@
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1574,14 +1574,14 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1669,14 +1669,14 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1764,14 +1764,14 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1859,14 +1859,14 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1954,14 +1954,14 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2049,14 +2049,14 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2144,14 +2144,14 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2239,14 +2239,14 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2334,13 +2334,13 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" s="5">
@@ -2429,13 +2429,13 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" s="5">
@@ -2524,13 +2524,13 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="5">
@@ -2619,13 +2619,13 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" s="5">
@@ -2714,14 +2714,14 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2809,14 +2809,14 @@
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2904,14 +2904,14 @@
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Ban new crude oil plants
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E195D9-0360-4576-AA72-E7FBED472E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FAE64A-13CE-4005-8BFB-2EA565AF1CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33585" yWindow="1950" windowWidth="21870" windowHeight="13605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31410" yWindow="2610" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -557,8 +557,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:AE21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1996,95 +1996,95 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0</v>
-      </c>
-      <c r="R16" s="2">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2">
-        <v>0</v>
-      </c>
-      <c r="T16" s="2">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
-        <v>0</v>
-      </c>
-      <c r="W16" s="2">
-        <v>0</v>
-      </c>
-      <c r="X16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="2">
-        <v>0</v>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
+        <v>1</v>
+      </c>
+      <c r="AE16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>